<commit_message>
Generate json from tasks and team excel files
</commit_message>
<xml_diff>
--- a/ExampleFiles/team.xlsx
+++ b/ExampleFiles/team.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B56DEAE-84CF-4E26-AB24-212D82F23C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E29763-BE4A-4BAA-A276-3D7618DBCBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6324" yWindow="2364" windowWidth="10848" windowHeight="6456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,13 +57,13 @@
     <t>Dave</t>
   </si>
   <si>
-    <t>2025-03-10;2025-03-15</t>
-  </si>
-  <si>
-    <t>2025-04-05;2025-04-10</t>
-  </si>
-  <si>
-    <t>2025-02-25;2025-02-28</t>
+    <t>2025-04-05;2025-04-10|</t>
+  </si>
+  <si>
+    <t>2025-02-25;2025-02-28|</t>
+  </si>
+  <si>
+    <t>2025-03-10;2025-03-15|2025-05-10;2025-05-15</t>
   </si>
 </sst>
 </file>
@@ -116,6 +116,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5156F39C-A57D-49CD-8981-173D65261D30}" name="Table1" displayName="Table1" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{5156F39C-A57D-49CD-8981-173D65261D30}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FCDF013B-522F-424B-BADC-9CEF21FEDF0C}" name="Team Name"/>
+    <tableColumn id="2" xr3:uid="{6FD6B03C-FF41-424E-B780-CE9F18124A33}" name="Developer Name"/>
+    <tableColumn id="3" xr3:uid="{739677C6-659D-4128-8D44-67677C3D3029}" name="Developer Vacation Date Intervals"/>
+    <tableColumn id="4" xr3:uid="{CF1E86B6-655B-4B30-A05A-C620D03124E5}" name="Daily Work Hours"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,15 +397,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -417,7 +430,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -442,7 +455,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -456,7 +469,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -464,5 +477,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>